<commit_message>
Added Animals to Spreadsheet
</commit_message>
<xml_diff>
--- a/Resources/Documents/Spread.xlsx
+++ b/Resources/Documents/Spread.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasdair\Desktop\University\Year 2\2nd Trimester\Programming for Unity\God Game\repository\Resources\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b00330023\Desktop\University\3D Game\god-game\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="89">
   <si>
     <t>Base Entity</t>
   </si>
@@ -286,12 +286,21 @@
   </si>
   <si>
     <t>Icon</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Tiger</t>
+  </si>
+  <si>
+    <t>Leopard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -486,327 +495,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="228">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="176">
     <dxf>
       <fill>
         <patternFill>
@@ -822,66 +511,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -889,6 +518,400 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="7"/>
@@ -2119,477 +2142,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3395,10 +2947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3538,7 +3090,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>32</v>
@@ -3572,13 +3124,13 @@
         <v>61</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>32</v>
@@ -3749,129 +3301,129 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="20" t="s">
+      <c r="B21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>32</v>
@@ -3882,7 +3434,7 @@
       <c r="D26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E26" s="21" t="s">
         <v>32</v>
       </c>
       <c r="F26" s="20" t="s">
@@ -3891,7 +3443,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>32</v>
@@ -3911,240 +3463,240 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="20" t="s">
+      <c r="B31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="16"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="B36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="B37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="B38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="B39" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="16"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="16"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" s="21" t="s">
         <v>32</v>
@@ -4155,7 +3707,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B44" s="12" t="s">
         <v>32</v>
@@ -4170,12 +3722,12 @@
         <v>32</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B45" s="12" t="s">
         <v>32</v>
@@ -4195,7 +3747,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B46" s="12" t="s">
         <v>32</v>
@@ -4215,109 +3767,109 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="B50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="16"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="16"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>32</v>
@@ -4337,7 +3889,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>32</v>
@@ -4348,16 +3900,16 @@
       <c r="D55" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E55" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="12" t="s">
+      <c r="E55" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>32</v>
@@ -4377,7 +3929,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B57" s="12" t="s">
         <v>32</v>
@@ -4397,7 +3949,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B58" s="12" t="s">
         <v>32</v>
@@ -4408,435 +3960,503 @@
       <c r="D58" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E58" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F58" s="20" t="s">
+      <c r="E58" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="B62" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="B63" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E61" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F61" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="B64" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+      <c r="E66"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="16"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D66" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E66" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F66" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D67" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E67" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F67" s="21" t="s">
-        <v>32</v>
-      </c>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
+      <c r="D67" s="16"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="16"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B68" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D68" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F68" s="23" t="s">
+      <c r="B71" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="23" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B22:E22 B32:E32 B64:E64 B47 F1 B69:E1048576 B39:E39 B65 B1:E4 B40:D40 D47:E47 D65">
-    <cfRule type="cellIs" dxfId="173" priority="157" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="158" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50:E50 B51 B60:B61 B53 D53 D60 D51 D61:E61">
-    <cfRule type="cellIs" dxfId="171" priority="155" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="156" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="169" priority="127" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="168" priority="128" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33 D33">
-    <cfRule type="cellIs" dxfId="167" priority="153" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="154" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B7 B11 D11 D5:D7">
-    <cfRule type="cellIs" dxfId="165" priority="151" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="152" operator="equal">
+  <conditionalFormatting sqref="B25:E25 B35:E35 B67:E67 B50 F1 B72:E1048576 B42:E42 B68 B1:E4 B43:D43 D50:E50 D68">
+    <cfRule type="cellIs" dxfId="175" priority="179" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="180" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53:E53 B54 B63:B64 B56 D56 D63 D54 D64:E64">
+    <cfRule type="cellIs" dxfId="173" priority="177" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="172" priority="178" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" dxfId="171" priority="149" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="170" priority="150" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36 D36">
-    <cfRule type="cellIs" dxfId="163" priority="149" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="150" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19 D19">
-    <cfRule type="cellIs" dxfId="161" priority="147" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="148" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29 D29">
-    <cfRule type="cellIs" dxfId="159" priority="145" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="146" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23 D23">
-    <cfRule type="cellIs" dxfId="157" priority="143" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="175" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="176" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:B7 B11 D11 D5:D6">
+    <cfRule type="cellIs" dxfId="167" priority="173" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="166" priority="174" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39 D39">
+    <cfRule type="cellIs" dxfId="165" priority="171" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="164" priority="172" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22 D22">
+    <cfRule type="cellIs" dxfId="163" priority="169" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="170" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32 D32">
+    <cfRule type="cellIs" dxfId="161" priority="167" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="160" priority="168" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26 D26">
+    <cfRule type="cellIs" dxfId="159" priority="165" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="158" priority="166" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="157" priority="163" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="164" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="155" priority="141" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="142" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="cellIs" dxfId="153" priority="139" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="140" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="151" priority="137" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="161" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="162" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="cellIs" dxfId="153" priority="159" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="160" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63">
+    <cfRule type="cellIs" dxfId="151" priority="157" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="158" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7 E11">
+    <cfRule type="cellIs" dxfId="149" priority="155" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="156" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="147" priority="153" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="154" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="145" priority="151" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="152" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A22">
+    <cfRule type="expression" dxfId="143" priority="147">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="142" priority="148">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A26:A32">
+    <cfRule type="expression" dxfId="141" priority="145">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="140" priority="146">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:A39">
+    <cfRule type="expression" dxfId="139" priority="143">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="138" priority="144">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:A50">
+    <cfRule type="expression" dxfId="137" priority="141">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="136" priority="142">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:A64">
+    <cfRule type="expression" dxfId="135" priority="139">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="134" priority="140">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68:A71">
+    <cfRule type="expression" dxfId="133" priority="137">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="132" priority="138">
+      <formula>MOD(ROW(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="cellIs" dxfId="131" priority="135" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="136" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B62 D62">
+    <cfRule type="cellIs" dxfId="129" priority="133" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="134" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule type="cellIs" dxfId="127" priority="131" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="132" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60:B61 D60:D61">
+    <cfRule type="cellIs" dxfId="125" priority="129" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="130" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="cellIs" dxfId="149" priority="135" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="136" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5:E7 E11">
-    <cfRule type="cellIs" dxfId="147" priority="133" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="134" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="145" priority="131" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="132" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="143" priority="129" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="130" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A19">
-    <cfRule type="expression" dxfId="141" priority="125">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="140" priority="126">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A29">
-    <cfRule type="expression" dxfId="139" priority="123">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="138" priority="124">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33:A36">
-    <cfRule type="expression" dxfId="137" priority="121">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="136" priority="122">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40:A47">
-    <cfRule type="expression" dxfId="135" priority="119">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="134" priority="120">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:A61">
-    <cfRule type="expression" dxfId="133" priority="117">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="132" priority="118">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:A68">
-    <cfRule type="expression" dxfId="131" priority="115">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="130" priority="116">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
-    <cfRule type="cellIs" dxfId="129" priority="113" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="127" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="128" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule type="cellIs" dxfId="121" priority="125" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="126" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="cellIs" dxfId="119" priority="121" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="122" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="cellIs" dxfId="117" priority="117" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="118" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59 D59">
-    <cfRule type="cellIs" dxfId="127" priority="111" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="112" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="cellIs" dxfId="125" priority="109" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="110" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B57:B58 D57:D58">
-    <cfRule type="cellIs" dxfId="123" priority="107" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="108" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
-    <cfRule type="cellIs" dxfId="121" priority="105" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="106" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="cellIs" dxfId="119" priority="103" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="104" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
-    <cfRule type="cellIs" dxfId="117" priority="99" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="100" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
-    <cfRule type="cellIs" dxfId="115" priority="95" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="96" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56 D56">
-    <cfRule type="cellIs" dxfId="113" priority="101" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="102" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="cellIs" dxfId="111" priority="91" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="92" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B54 D54">
+    <cfRule type="cellIs" dxfId="115" priority="123" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="124" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" dxfId="113" priority="113" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="114" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57 D57">
+    <cfRule type="cellIs" dxfId="111" priority="119" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="120" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:E10">
     <cfRule type="cellIs" dxfId="109" priority="97" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -4844,359 +4464,435 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:E10">
-    <cfRule type="cellIs" dxfId="107" priority="75" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="76" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52 D52">
-    <cfRule type="cellIs" dxfId="105" priority="93" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="94" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="103" priority="67" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="68" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B46 D41:D46">
-    <cfRule type="cellIs" dxfId="101" priority="89" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="90" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41:E46">
-    <cfRule type="cellIs" dxfId="99" priority="87" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="88" operator="equal">
+  <conditionalFormatting sqref="B55 D55">
+    <cfRule type="cellIs" dxfId="107" priority="115" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="116" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="cellIs" dxfId="105" priority="89" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="90" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:B49 D44:D49">
+    <cfRule type="cellIs" dxfId="103" priority="111" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="112" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44:E49">
+    <cfRule type="cellIs" dxfId="101" priority="109" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="110" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14 D14">
-    <cfRule type="cellIs" dxfId="97" priority="85" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="107" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="108" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="95" priority="83" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="105" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="106" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12 D12">
-    <cfRule type="cellIs" dxfId="93" priority="81" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="103" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="104" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="91" priority="79" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="101" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="102" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10 D8:D10">
-    <cfRule type="cellIs" dxfId="89" priority="77" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="99" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="100" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="87" priority="63" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="64" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34 D34">
-    <cfRule type="cellIs" dxfId="85" priority="73" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="74" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35 D35">
-    <cfRule type="cellIs" dxfId="81" priority="69" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="85" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="86" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37 D37">
+    <cfRule type="cellIs" dxfId="87" priority="95" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="96" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" dxfId="85" priority="93" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="94" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38 D38">
+    <cfRule type="cellIs" dxfId="83" priority="91" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="92" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13 D13">
-    <cfRule type="cellIs" dxfId="79" priority="65" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F19 F51:F54 F23:F29 F33:F36 F40:F47 F56:F61">
-    <cfRule type="cellIs" dxfId="77" priority="61" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F50">
-    <cfRule type="cellIs" dxfId="76" priority="57" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="58" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F64">
-    <cfRule type="cellIs" dxfId="74" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="56" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="72" priority="53" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="54" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F32">
-    <cfRule type="cellIs" dxfId="70" priority="51" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="52" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="68" priority="49" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="50" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F65 F68">
-    <cfRule type="cellIs" dxfId="66" priority="47" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="48" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F54 F56:F65 F68:F1048576">
-    <cfRule type="cellIs" dxfId="64" priority="46" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B18 D16:E18">
-    <cfRule type="cellIs" dxfId="63" priority="45" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16:B18 D16:E18">
-    <cfRule type="cellIs" dxfId="62" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="87" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="88" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F17 F54:F57 F26:F32 F36:F39 F43:F50 F59:F64 F21:F22">
+    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F53">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="80" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F67">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="78" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="76" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="cellIs" dxfId="72" priority="73" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="74" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="70" priority="71" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="72" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F68 F71">
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="70" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F17 F59:F68 F71:F1048576 F21:F57">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B17 D16:E17 D21:E21 B21">
+    <cfRule type="cellIs" dxfId="65" priority="67" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B17 D16:E17 D21:E21 B21">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15 D15:E15">
-    <cfRule type="cellIs" dxfId="61" priority="42" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="43" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24:B28 D24:E28">
-    <cfRule type="cellIs" dxfId="59" priority="40" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="41" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55 D55:F55">
-    <cfRule type="cellIs" dxfId="57" priority="38" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="39" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F68">
-    <cfRule type="cellIs" dxfId="55" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="64" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="65" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:B31 D27:E31">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58 D58:F58">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F71">
+    <cfRule type="cellIs" dxfId="57" priority="59" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="58" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71">
+    <cfRule type="cellIs" dxfId="53" priority="55" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D71">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B71">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B71">
+    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B71">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="54" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="52" priority="34" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="51" priority="33" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="cellIs" dxfId="50" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="cellIs" dxfId="48" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="cellIs" dxfId="47" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="46" priority="27" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="44" priority="26" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
-    <cfRule type="cellIs" dxfId="43" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="42" priority="23" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="24" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="cellIs" dxfId="40" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="cellIs" dxfId="39" priority="20" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66 D66:F66">
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67 D67:F67">
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C61">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C47">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C36">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65:C68">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23:C29">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C19">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69 D69:E69">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B70 D70:F70">
+    <cfRule type="cellIs" dxfId="37" priority="35" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C63">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:C49">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36:C38">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C70">
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26:C31">
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C17 C21">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F69">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:F20">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:F20">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:F18">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:F18">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5380,10 +5076,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 A10:A21 A4:A8">
-    <cfRule type="expression" dxfId="33" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Reworked Breeding Mechanic and New AI System
-Entities only breed with the same species.
-Entities can now selectively breed new species.
-AI System works on a priority basis, with room for expansion
-Modelled & Imported New Entities: Fir Tree, Oak Tree, Elder Tree, Dead Tree, Deer, Wolf, and Boar
</commit_message>
<xml_diff>
--- a/Resources/Documents/Spread.xlsx
+++ b/Resources/Documents/Spread.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b00330023\Desktop\University\3D Game\god-game\Resources\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alasdair\Desktop\University\Year 2\2nd Trimester\Programming for Unity\God Game\rep\god-game\Resources\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="92">
   <si>
     <t>Base Entity</t>
   </si>
@@ -295,12 +295,21 @@
   </si>
   <si>
     <t>Leopard</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Boar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -497,6 +506,26 @@
   </cellStyles>
   <dxfs count="176">
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
@@ -531,26 +560,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2949,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,13 +3153,13 @@
         <v>60</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>32</v>
@@ -3164,13 +3173,13 @@
         <v>19</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>32</v>
@@ -3381,16 +3390,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E22" s="22" t="s">
         <v>32</v>
@@ -3710,13 +3719,13 @@
         <v>50</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44" s="21" t="s">
         <v>32</v>
@@ -3750,13 +3759,13 @@
         <v>56</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E46" s="21" t="s">
         <v>32</v>
@@ -3770,13 +3779,13 @@
         <v>55</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E47" s="21" t="s">
         <v>32</v>
@@ -4877,22 +4886,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:F20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:F20">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:F18">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4905,7 +4914,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4937,6 +4946,9 @@
       <c r="B2" t="s">
         <v>82</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -4975,7 +4987,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -5076,10 +5088,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2 A10:A21 A4:A8">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5089,10 +5101,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="K2:U4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5100,40 +5112,24 @@
     <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="K2" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="11:21" x14ac:dyDescent="0.25">
-      <c r="M4" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="U4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>